<commit_message>
Improved account sign up
- Added regex to check password strength
- Faculty lists expanded
</commit_message>
<xml_diff>
--- a/server/services/DummyCSV/faculties.xlsx
+++ b/server/services/DummyCSV/faculties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonng/Desktop/booKING-main/server/DummyCSV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonng/Desktop/booKING/server/services/DummyCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DEA4CF-9607-524F-BEC7-886D9D5130CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1E713F-503B-F943-9760-0D14BFB0C5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{7CDF45CC-41A3-204B-BF0B-7A172C9467F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>facultyID</t>
   </si>
@@ -57,7 +57,76 @@
     <t>Faculty of Arts and Social Sciences</t>
   </si>
   <si>
-    <t>Others</t>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Business School</t>
+  </si>
+  <si>
+    <t>SCALE</t>
+  </si>
+  <si>
+    <t>School of Continuing and Lifelong Education</t>
+  </si>
+  <si>
+    <t>Dentistry</t>
+  </si>
+  <si>
+    <t>Faculty of Dentistry</t>
+  </si>
+  <si>
+    <t>SDE</t>
+  </si>
+  <si>
+    <t>School of Design &amp; Environment</t>
+  </si>
+  <si>
+    <t>FoE</t>
+  </si>
+  <si>
+    <t>Faculty of Engineering</t>
+  </si>
+  <si>
+    <t>ISEP</t>
+  </si>
+  <si>
+    <t>Integrative Sciences and Engineering Programme</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Faculty of Law</t>
+  </si>
+  <si>
+    <t>Yong Loo Lin School of Medicine</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Yong Siew Toh Conservatory of Music</t>
+  </si>
+  <si>
+    <t>Public Health</t>
+  </si>
+  <si>
+    <t>Saw See Hock School of Public Health</t>
+  </si>
+  <si>
+    <t>Public Policy</t>
+  </si>
+  <si>
+    <t>Lee Kuan Yew School of Public Policy</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Faculty of Science</t>
   </si>
 </sst>
 </file>
@@ -409,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2A1B1D-0303-8B45-8E4F-1CB093D1DEC2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -447,10 +516,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -458,10 +527,131 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More edits to dummy csv files
</commit_message>
<xml_diff>
--- a/server/services/DummyCSV/faculties.xlsx
+++ b/server/services/DummyCSV/faculties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonng/Desktop/booKING/server/services/DummyCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1E713F-503B-F943-9760-0D14BFB0C5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95289309-EB65-CA4E-A8DC-75512278EBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{7CDF45CC-41A3-204B-BF0B-7A172C9467F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>facultyID</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Faculty of Science</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2A1B1D-0303-8B45-8E4F-1CB093D1DEC2}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -654,6 +657,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>